<commit_message>
latest with GUI connection
</commit_message>
<xml_diff>
--- a/Meeting-Manager/data.xlsx
+++ b/Meeting-Manager/data.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1068,6 +1068,1413 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2134</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2134</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2134</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00:00:00.000 --&gt; 00:00:02.000
+Kasim Alam
+Hey Pourna.
+00:00:03.000 --&gt; 00:00:05.000
+Pourna Sengupta
+Hey Kasim.
+00:00:06.0 --&gt; 00:00:08.0
+Kasim Alam
+Let's get this meeting started.
+00:00:09.0 --&gt; 00:00:11.0
+Pourna Sengupta
+Sounds good.
+00:00:12.0 --&gt; 00:00:14.0
+Kasim Alam
+We need to have a call tomorrow at noon with Pradeep Thelakkat to discuss the meeting manager bot.
+00:00:15.0 --&gt; 00:00:17.0
+Pourna Sengupta
+I agree. We should definitely get on that. We also need to create a user story for creating the bot.
+00:00:18.0 --&gt; 00:00:20.0
+Kasim Alam
+True.
+00:00:21.0 --&gt; 00:00:23.0
+Pourna Sengupta
+Let's create a group chat with Pradeep Thelakkat in the meantime so that we can discuss.
+00:00:24.0 --&gt; 00:00:26.0
+Kasim Alam
+That's a good idea. So to recap, we need to create a meeting with Pradeep, create a group chat with Pradeep and create a user story for the bot creation.
+00:00:27.0 --&gt; 00:00:29.0
+Pourna Sengupta
+That's right.
+00:00:30.0 --&gt; 00:00:32.0
+Kasim Alam
+Sounds good, that's all I wanted to cover today. Take care.
+00:00:33.0 --&gt; 00:00:35.0
+Pourna Sengupta
+You too.
+</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>